<commit_message>
Legende in xls file
</commit_message>
<xml_diff>
--- a/mcmods.xlsx
+++ b/mcmods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Mods</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>Wichtig?</t>
+  </si>
+  <si>
+    <t>hoffentlich funktionstüchtig</t>
+  </si>
+  <si>
+    <t>nicht verfügbar</t>
+  </si>
+  <si>
+    <t>verfügbar</t>
+  </si>
+  <si>
+    <t>Legende</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -231,6 +243,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -511,19 +524,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G67"/>
+  <dimension ref="A3:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
@@ -545,8 +559,11 @@
       <c r="G3" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I3" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
@@ -558,8 +575,11 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
@@ -571,8 +591,11 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -582,8 +605,11 @@
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
@@ -596,7 +622,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -607,7 +633,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>31</v>
       </c>
@@ -620,7 +646,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>31</v>
       </c>
@@ -633,7 +659,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>31</v>
       </c>
@@ -646,7 +672,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -659,7 +685,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>31</v>
       </c>
@@ -672,7 +698,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -683,7 +709,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -696,7 +722,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
added betterMountHUD and updated Xaeros mods
</commit_message>
<xml_diff>
--- a/mcmods.xlsx
+++ b/mcmods.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Wichtig?</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>zoomify</t>
+  </si>
+  <si>
+    <t>bettermountHUD</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <dimension ref="A3:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +594,7 @@
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -603,11 +606,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -616,35 +617,35 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -657,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -670,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -683,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -692,9 +693,11 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -703,11 +706,9 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -720,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -733,7 +734,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -742,9 +743,11 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -755,33 +758,31 @@
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -794,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -803,9 +804,11 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B23" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -816,33 +819,31 @@
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -855,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -868,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -876,6 +877,19 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67">
         <f>SUM(C42:C57)</f>

</xml_diff>

<commit_message>
added Better f3 for 1.21.11
</commit_message>
<xml_diff>
--- a/mcmods.xlsx
+++ b/mcmods.xlsx
@@ -523,7 +523,7 @@
   <dimension ref="A3:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
+      <c r="G5" s="11"/>
       <c r="I5" s="8" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
added Ferritcore, immediatly fast, entity culling, skinlayers 3d, shulkerbox tooltip
</commit_message>
<xml_diff>
--- a/mcmods.xlsx
+++ b/mcmods.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Wichtig?</t>
   </si>
@@ -138,6 +138,21 @@
   </si>
   <si>
     <t>bettermountHUD</t>
+  </si>
+  <si>
+    <t>entity culling</t>
+  </si>
+  <si>
+    <t>immediatly fast</t>
+  </si>
+  <si>
+    <t>ferritcore</t>
+  </si>
+  <si>
+    <t>shulkerbox tooltip</t>
+  </si>
+  <si>
+    <t>skinlayers 3d</t>
   </si>
 </sst>
 </file>
@@ -522,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,11 +682,9 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -684,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -697,7 +710,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -706,9 +719,11 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B15" s="6" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -721,7 +736,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -734,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -743,11 +758,9 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -756,9 +769,11 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B19" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -767,22 +782,24 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B20" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -791,11 +808,9 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A22" s="5"/>
       <c r="B22" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -804,22 +819,20 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="5"/>
       <c r="B23" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -830,20 +843,20 @@
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="10"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -856,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -869,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -878,11 +891,9 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A29" s="5"/>
       <c r="B29" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -890,6 +901,69 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
+    <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C67">
         <f>SUM(C42:C57)</f>

</xml_diff>